<commit_message>
regenerate test results source data after fixing scripts
</commit_message>
<xml_diff>
--- a/results/VSD/source_data/test_results_table_initialize_mean_sd_single_col.xlsx
+++ b/results/VSD/source_data/test_results_table_initialize_mean_sd_single_col.xlsx
@@ -495,17 +495,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.353 (0.353)</t>
+          <t>0.353 (0.056)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.330 (0.330)</t>
+          <t>0.330 (0.037)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0.184 (0.184)</t>
+          <t>0.184 (0.042)</t>
         </is>
       </c>
     </row>
@@ -518,17 +518,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.390 (0.390)</t>
+          <t>0.390 (0.009)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.346 (0.346)</t>
+          <t>0.346 (0.009)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0.194 (0.194)</t>
+          <t>0.194 (0.001)</t>
         </is>
       </c>
     </row>
@@ -541,17 +541,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.453 (0.453)</t>
+          <t>0.453 (0.020)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.404 (0.404)</t>
+          <t>0.404 (0.019)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.197 (0.197)</t>
+          <t>0.197 (0.006)</t>
         </is>
       </c>
     </row>
@@ -564,17 +564,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.467 (0.467)</t>
+          <t>0.467 (0.018)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.418 (0.418)</t>
+          <t>0.418 (0.019)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.204 (0.204)</t>
+          <t>0.204 (0.004)</t>
         </is>
       </c>
     </row>
@@ -591,12 +591,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.124 (0.124)</t>
+          <t>0.124 (0.085)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.137 (0.137)</t>
+          <t>0.137 (0.101)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -614,17 +614,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.128 (0.128)</t>
+          <t>0.128 (0.081)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.150 (0.150)</t>
+          <t>0.150 (0.087)</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.014 (0.014)</t>
+          <t>0.014 (0.010)</t>
         </is>
       </c>
     </row>
@@ -637,17 +637,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0.208 (0.208)</t>
+          <t>0.208 (0.001)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.238 (0.238)</t>
+          <t>0.238 (0.002)</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0.006 (0.006)</t>
+          <t>0.006 (0.007)</t>
         </is>
       </c>
     </row>
@@ -660,17 +660,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0.300 (0.300)</t>
+          <t>0.300 (0.049)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.301 (0.301)</t>
+          <t>0.301 (0.045)</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0.106 (0.106)</t>
+          <t>0.106 (0.025)</t>
         </is>
       </c>
     </row>

</xml_diff>